<commit_message>
age data excel but better
</commit_message>
<xml_diff>
--- a/sterlingdata.xlsx
+++ b/sterlingdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10808"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65BF505A-501B-C440-9E89-9A1202B3ECB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB805CF-C24E-8540-B570-C5F7E52ABE13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2072,9 +2072,6 @@
     <t>85&gt;</t>
   </si>
   <si>
-    <t>5 to 9</t>
-  </si>
-  <si>
     <t>10 to 14</t>
   </si>
   <si>
@@ -2103,6 +2100,9 @@
   </si>
   <si>
     <t>75 to 84</t>
+  </si>
+  <si>
+    <t>05 to 09</t>
   </si>
 </sst>
 </file>
@@ -2529,7 +2529,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A20" sqref="A20"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2814,7 +2814,7 @@
     </row>
     <row r="9" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>684</v>
+        <v>694</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>51</v>
@@ -2855,7 +2855,7 @@
     </row>
     <row r="10" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>61</v>
@@ -2896,7 +2896,7 @@
     </row>
     <row r="11" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>70</v>
@@ -2937,7 +2937,7 @@
     </row>
     <row r="12" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>79</v>
@@ -2978,7 +2978,7 @@
     </row>
     <row r="13" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>89</v>
@@ -3019,7 +3019,7 @@
     </row>
     <row r="14" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>99</v>
@@ -3060,7 +3060,7 @@
     </row>
     <row r="15" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>109</v>
@@ -3101,7 +3101,7 @@
     </row>
     <row r="16" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>118</v>
@@ -3142,7 +3142,7 @@
     </row>
     <row r="17" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>127</v>
@@ -3183,7 +3183,7 @@
     </row>
     <row r="18" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>136</v>
@@ -3224,7 +3224,7 @@
     </row>
     <row r="19" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>145</v>

</xml_diff>

<commit_message>
finished demographics for age, poverty by sex and age, and median income as well as their respective excel sheets.
</commit_message>
<xml_diff>
--- a/sterlingdata.xlsx
+++ b/sterlingdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10808"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB805CF-C24E-8540-B570-C5F7E52ABE13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB7F963-DB61-2D44-B3E9-C65240C7000F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2178,11 +2178,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1" indent="4"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2542,24 +2542,24 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7" t="s">
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
     </row>
     <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -2813,7 +2813,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>694</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -2854,7 +2854,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>684</v>
       </c>
       <c r="B10" s="1" t="s">

</xml_diff>